<commit_message>
Aula do dia 28/10
</commit_message>
<xml_diff>
--- a/PesquisaOperacional/Aula26/Pasta1.xlsx
+++ b/PesquisaOperacional/Aula26/Pasta1.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>x1</t>
   </si>
@@ -84,12 +84,6 @@
     <t>RHS</t>
   </si>
   <si>
-    <t>Preço-Sombra é o quanto a função objetivo aumenta ou diminui</t>
-  </si>
-  <si>
-    <t>Custo reduzido é o total que seu coeficiente da função objetivo deve melhorar para que ela deixa de ser zero</t>
-  </si>
-  <si>
     <t>Microsoft Excel 16.0 Relatório de Sensibilidade</t>
   </si>
   <si>
@@ -184,13 +178,39 @@
   </si>
   <si>
     <t>Restrição 3 LHS</t>
+  </si>
+  <si>
+    <t>Preço sombra é a alteração que irá ocorrer na função objetivo ao adicionar ou diminuir um valor em alguma constante de restrição</t>
+  </si>
+  <si>
+    <t>Reduzido custo é a alteração(Penalização) que será feito em uma variavel para que ela se torne básica</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <r>
+      <t>Podem ser calculados para os bens e serviços que não tenham um preço</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> de mercado, por exemplo por serem fixados por um governo.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +233,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -567,7 +593,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:H12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,82 +608,72 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="H7" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="H8" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" s="2">
         <v>1.1428571428571428</v>
@@ -677,10 +693,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -700,10 +716,10 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="3">
         <v>2.4285714285714284</v>
@@ -723,57 +739,57 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="E15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="G15" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" s="2">
         <v>200</v>
@@ -793,10 +809,10 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" s="2">
         <v>179.99999999999997</v>
@@ -816,10 +832,10 @@
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D18" s="3">
         <v>157.14285714285711</v>
@@ -844,10 +860,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +871,7 @@
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -866,7 +882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>21</v>
       </c>
@@ -877,7 +893,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -891,7 +907,7 @@
         <v>2.4285714285714284</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -899,22 +915,16 @@
         <f>SUMPRODUCT(B3:D3,B2:D2)</f>
         <v>60.428571428571423</v>
       </c>
-      <c r="L4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
       </c>
-      <c r="L5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -935,7 +945,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -956,7 +966,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -975,6 +985,27 @@
       </c>
       <c r="F8">
         <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>